<commit_message>
studentgrades dataframe builds with repeated courses taken
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9147DC-D6B9-4C97-8FBA-B2D6A5D7689E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FF9BA2-7FBF-4DAE-8C0F-41CEE19CCCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -86,7 +86,7 @@
     <t>08/05/2024</t>
   </si>
   <si>
-    <t>more data formatting</t>
+    <t>more data formatting, finished framework for building studentgrades df</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -594,7 +594,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
fixed bugs with creating studentgrades:
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FF9BA2-7FBF-4DAE-8C0F-41CEE19CCCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B6E2A3-C8A2-4B38-B1FC-713AE83C3DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>more data formatting, finished framework for building studentgrades df</t>
+  </si>
+  <si>
+    <t>09/05/2024</t>
+  </si>
+  <si>
+    <t>fixed bugs</t>
   </si>
 </sst>
 </file>
@@ -491,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -594,10 +600,21 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made new df for majors and minors, no combined majors yet
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B6E2A3-C8A2-4B38-B1FC-713AE83C3DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BF4669-EEB6-4A09-BFED-40B13BF22583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -50,49 +50,25 @@
     <t>Links</t>
   </si>
   <si>
-    <t>25/04/2024</t>
-  </si>
-  <si>
     <t>Daniel setting me up</t>
   </si>
   <si>
-    <t>30/04/2024</t>
-  </si>
-  <si>
     <t>First meeting with Irene to talk over project</t>
   </si>
   <si>
-    <t>02/05/2024</t>
-  </si>
-  <si>
     <t>trying out xgboosted model</t>
   </si>
   <si>
-    <t>03/05/2024</t>
-  </si>
-  <si>
-    <t>05/05/2024</t>
-  </si>
-  <si>
-    <t>06/05/2024</t>
-  </si>
-  <si>
-    <t>07/05/2024</t>
-  </si>
-  <si>
     <t>meeting, trying to format data</t>
   </si>
   <si>
-    <t>08/05/2024</t>
-  </si>
-  <si>
     <t>more data formatting, finished framework for building studentgrades df</t>
   </si>
   <si>
-    <t>09/05/2024</t>
-  </si>
-  <si>
     <t>fixed bugs</t>
+  </si>
+  <si>
+    <t>adding majors and minors to studentgrades, no combined majors yet</t>
   </si>
 </sst>
 </file>
@@ -159,10 +135,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,124 +473,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.86328125" customWidth="1"/>
     <col min="2" max="2" width="11.59765625" customWidth="1"/>
-    <col min="3" max="3" width="2.1328125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="2.1328125" style="3" customWidth="1"/>
     <col min="4" max="4" width="43.1328125" customWidth="1"/>
     <col min="5" max="5" width="27.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" s="4">
+        <v>45407</v>
       </c>
       <c r="B2">
         <v>1.5</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
+      <c r="A3" s="4">
+        <v>45412</v>
       </c>
       <c r="B3">
         <v>0.5</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>8</v>
+      <c r="A4" s="4">
+        <v>45414</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>10</v>
+      <c r="A5" s="4">
+        <v>45415</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>11</v>
+      <c r="A6" s="4">
+        <v>45417</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>12</v>
+      <c r="A7" s="4">
+        <v>45418</v>
       </c>
       <c r="B7">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>13</v>
+      <c r="A8" s="4">
+        <v>45419</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>15</v>
+      <c r="A9" s="4">
+        <v>45420</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>17</v>
+      <c r="A10" s="4">
+        <v>45421</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="4">
+        <v>45422</v>
+      </c>
+      <c r="B11">
+        <v>2.5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
combined majors add to student grades df
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BF4669-EEB6-4A09-BFED-40B13BF22583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5627DCA8-9C8E-46B4-901B-ADBEB90B6956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="5400" yWindow="0" windowWidth="16200" windowHeight="8295" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
     <t>fixed bugs</t>
   </si>
   <si>
-    <t>adding majors and minors to studentgrades, no combined majors yet</t>
+    <t>adding majors and minors to studentgrades, combined majors now work</t>
   </si>
 </sst>
 </file>
@@ -473,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -598,10 +598,15 @@
         <v>45422</v>
       </c>
       <c r="B11">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="4">
+        <v>45425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EDA started, empty columns found..
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5627DCA8-9C8E-46B4-901B-ADBEB90B6956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182FFBDF-E80E-4060-B83D-312977B067F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="0" windowWidth="16200" windowHeight="8295" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>adding majors and minors to studentgrades, combined majors now work</t>
+  </si>
+  <si>
+    <t>finished and pushed student major/minor, need to ask about other options… Now it’s time to find and fix bugs of empty columns…</t>
   </si>
 </sst>
 </file>
@@ -133,12 +136,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,7 +482,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -604,9 +610,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>45425</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying out random forests and GBM on basic math/stat courses
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8452ED7A-10C1-4F03-BE58-FB9FF7D92F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDA0B52-3206-40A2-B2F9-B9D2ECBD6FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>finished and pushed student major/minor, need to ask about other options… Now it’s time to find and fix bugs of empty columns…</t>
+  </si>
+  <si>
+    <t>trying out random forests, missForest, and GBM</t>
   </si>
 </sst>
 </file>
@@ -479,22 +482,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.86328125" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" customWidth="1"/>
-    <col min="3" max="3" width="2.1328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.1328125" customWidth="1"/>
-    <col min="5" max="5" width="27.59765625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -520,7 +523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -531,7 +534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -542,7 +545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -550,7 +553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -558,7 +561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -566,7 +569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -577,7 +580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -588,7 +591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -599,7 +602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -610,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -619,6 +622,17 @@
       </c>
       <c r="D12" s="5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>45426</v>
+      </c>
+      <c r="B13">
+        <v>2.5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying GBM on courses of the same year level and below.. currently breaking slightly
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDA0B52-3206-40A2-B2F9-B9D2ECBD6FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09970365-4D3D-4733-92D8-D232604B055C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
         <v>45426</v>
       </c>
       <c r="B13">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
removing future course attempts from prediction
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09970365-4D3D-4733-92D8-D232604B055C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1240788F-923A-4FCE-B883-FC1B02EED337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>trying out random forests, missForest, and GBM</t>
+  </si>
+  <si>
+    <t>removed all "future" courses (aka retries at the same course AND courses of a higher year level)</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>compare relevancies between courses| create a multi output regression model</t>
   </si>
 </sst>
 </file>
@@ -482,22 +491,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="2.1328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="43.1328125" customWidth="1"/>
+    <col min="5" max="5" width="27.59765625" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,8 +521,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -523,7 +536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -534,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -545,7 +558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -553,7 +566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -561,7 +574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -569,7 +582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -580,7 +593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -591,7 +604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -602,7 +615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -613,7 +626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -624,19 +637,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A14" s="4">
+        <v>45427</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding metrics to evaluate model
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1240788F-923A-4FCE-B883-FC1B02EED337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF810C6-03BC-4D4C-A1C2-9F1E1060815E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <t>TODO</t>
   </si>
   <si>
-    <t>compare relevancies between courses| create a multi output regression model</t>
+    <t xml:space="preserve">compare relevancies between courses| create a multi output regression model </t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -653,7 +653,7 @@
         <v>45427</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
ironing out bugs and prediction pipeline inconsistencies
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF810C6-03BC-4D4C-A1C2-9F1E1060815E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B1B4DD-9447-418D-B215-23D08A537463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t xml:space="preserve">compare relevancies between courses| create a multi output regression model </t>
+  </si>
+  <si>
+    <t>added prediction metrics</t>
+  </si>
+  <si>
+    <t>Look into other and all metrics, the potential of RF's again</t>
   </si>
 </sst>
 </file>
@@ -491,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -662,6 +668,22 @@
         <v>15</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="4">
+        <v>45428</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tried conf matrix, not working..
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B1B4DD-9447-418D-B215-23D08A537463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FE6716-C0D1-4969-9F11-FE65F3A90693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Look into other and all metrics, the potential of RF's again</t>
+  </si>
+  <si>
+    <t>Looking into confusion matrices to aid in precision</t>
   </si>
 </sst>
 </file>
@@ -154,13 +157,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -499,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -508,7 +514,7 @@
     <col min="1" max="1" width="12.86328125" customWidth="1"/>
     <col min="2" max="2" width="11.59765625" customWidth="1"/>
     <col min="3" max="3" width="2.1328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.1328125" customWidth="1"/>
+    <col min="4" max="4" width="43.1328125" style="5" customWidth="1"/>
     <col min="5" max="5" width="27.59765625" customWidth="1"/>
     <col min="6" max="6" width="31.33203125" customWidth="1"/>
   </cols>
@@ -521,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -538,7 +544,7 @@
       <c r="B2">
         <v>1.5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -549,7 +555,7 @@
       <c r="B3">
         <v>0.5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -560,7 +566,7 @@
       <c r="B4">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -595,18 +601,18 @@
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -617,18 +623,18 @@
       <c r="B10">
         <v>4</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -650,7 +656,7 @@
       <c r="B13">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -673,13 +679,22 @@
         <v>45428</v>
       </c>
       <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="4">
+        <v>45429</v>
+      </c>
+      <c r="B16">
         <v>5</v>
       </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D16" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="F16" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
trying larger training subset
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FE6716-C0D1-4969-9F11-FE65F3A90693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A71CD91-D804-4C50-BB75-E4638CC2A974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -92,7 +92,10 @@
     <t>Look into other and all metrics, the potential of RF's again</t>
   </si>
   <si>
-    <t>Looking into confusion matrices to aid in precision</t>
+    <t xml:space="preserve">Confusion matrix only useful for prediction, </t>
+  </si>
+  <si>
+    <t>Adding in BA student to widen the model training pool</t>
   </si>
 </sst>
 </file>
@@ -503,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -690,13 +693,24 @@
         <v>45429</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="4">
+        <v>45430</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new student grades df without course repitition
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A71CD91-D804-4C50-BB75-E4638CC2A974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92B1D7D-B4C3-48AD-99C3-6A3B2103AB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -95,7 +95,36 @@
     <t xml:space="preserve">Confusion matrix only useful for prediction, </t>
   </si>
   <si>
-    <t>Adding in BA student to widen the model training pool</t>
+    <t>Adding in BA student to widen the model training pool (reversed..)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Look into </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>best</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> grade student receives</t>
+    </r>
+  </si>
+  <si>
+    <t>Creating a new dataframe to save only newest grades student recieves, weights are based on rows in GBM</t>
   </si>
 </sst>
 </file>
@@ -506,23 +535,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.86328125" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" customWidth="1"/>
-    <col min="3" max="3" width="2.1328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.1328125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27.59765625" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +569,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -551,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -562,7 +591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -573,7 +602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -581,7 +610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -589,7 +618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -597,7 +626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -608,7 +637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -619,7 +648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -630,7 +659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -641,7 +670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -652,7 +681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -663,7 +692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -677,7 +706,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -688,7 +717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -702,15 +731,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>45431</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push before updating R
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF2886B-21B1-4265-9CA4-DCCDBD9C6CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DE5AE3-4A76-4776-BC36-B2B4CAE0BD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Work meeting, looking into many new papers and models (matrix factorization)</t>
+  </si>
+  <si>
+    <t>Researching NMF as a method of grade estimation</t>
   </si>
 </sst>
 </file>
@@ -538,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -770,6 +773,17 @@
         <v>22</v>
       </c>
     </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="4">
+        <v>45434</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MF working, not great
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CF5DFE-3DA6-44F2-819C-8614C5684D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792945DB-508E-4C3D-9667-B89780F783ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>Researching NMF as a method of grade estimation… cant handle NA's so nope. Now trying normal MF on STAT230 and its pre-reqs</t>
+  </si>
+  <si>
+    <t>MF working, similar mse, need to format new dataframe to train and test with</t>
+  </si>
+  <si>
+    <t>Finished mf using recosystem, not very good.. Looking to optimize</t>
   </si>
 </sst>
 </file>
@@ -544,23 +550,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.86328125" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" customWidth="1"/>
-    <col min="3" max="3" width="2.1328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.1328125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27.59765625" customWidth="1"/>
-    <col min="6" max="6" width="31.265625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -589,7 +595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -600,7 +606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -611,7 +617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -619,7 +625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -627,7 +633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -635,7 +641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -646,7 +652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -657,7 +663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -668,7 +674,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -679,7 +685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -690,7 +696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -701,7 +707,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -715,7 +721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -726,7 +732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -740,7 +746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -751,7 +757,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -765,7 +771,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -776,7 +782,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -790,12 +796,26 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
       <c r="B21">
         <v>7</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>45436</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
end of weekend changes
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792945DB-508E-4C3D-9667-B89780F783ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58C9062-E4BC-4E96-AF2A-105003C23AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="29385" yWindow="690" windowWidth="21600" windowHeight="11295" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -139,7 +139,13 @@
     <t>MF working, similar mse, need to format new dataframe to train and test with</t>
   </si>
   <si>
-    <t>Finished mf using recosystem, not very good.. Looking to optimize</t>
+    <t>Finished mf using recosystem, not very good.. Looking to optimize. Workday banking setup and courses.</t>
+  </si>
+  <si>
+    <t>Workday courses and minor testing</t>
+  </si>
+  <si>
+    <t>Changing course, no MF, at least not reguarly. Back to the drawing board.</t>
   </si>
 </sst>
 </file>
@@ -550,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,15 +813,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>45438</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pre FM and SVM
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58C9062-E4BC-4E96-AF2A-105003C23AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCCD2B6-FF74-4D20-8950-6484D0A75D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29385" yWindow="690" windowWidth="21600" windowHeight="11295" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Changing course, no MF, at least not reguarly. Back to the drawing board.</t>
+  </si>
+  <si>
+    <t>Looking into factorization machines and support vector machines. Trying to implement from scratch or use packages. Looking into the possibility of representing the student grades matrix as a binary matrix to use FMs. Planning to conduct a grid search on GBM parameters too.</t>
   </si>
 </sst>
 </file>
@@ -556,23 +559,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="2.1328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="43.1328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="27.59765625" customWidth="1"/>
+    <col min="6" max="6" width="31.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,7 +593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -601,7 +604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -612,7 +615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -623,7 +626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -631,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -639,7 +642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -647,7 +650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -658,7 +661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -669,7 +672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -680,7 +683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -691,7 +694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -702,7 +705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -713,7 +716,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -727,7 +730,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -738,7 +741,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -752,7 +755,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -763,7 +766,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -777,7 +780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -788,7 +791,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -802,7 +805,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
@@ -813,7 +816,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
@@ -824,7 +827,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
@@ -836,6 +839,17 @@
       </c>
       <c r="F23" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="4">
+        <v>45439</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing missForest and RF again
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCCD2B6-FF74-4D20-8950-6484D0A75D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64E32B2-FEBD-4F45-8CE7-F7823169AB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Looking into factorization machines and support vector machines. Trying to implement from scratch or use packages. Looking into the possibility of representing the student grades matrix as a binary matrix to use FMs. Planning to conduct a grid search on GBM parameters too.</t>
+  </si>
+  <si>
+    <t>Imputation into random forest seems to work the best…</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
@@ -852,6 +855,17 @@
         <v>29</v>
       </c>
     </row>
+    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="4">
+        <v>45440</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tried pairwise cor, no luck
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA206006-4FC9-42BE-90B8-CF8AAE77FDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C08764F-8A8F-4629-BCF6-7F30DC30F9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,7 +154,7 @@
     <t>Imputation into random forest seems to work the best…</t>
   </si>
   <si>
-    <t xml:space="preserve">Meeting </t>
+    <t>Meeting. Tried pairwise correlation, high cor on odd subjects (eg. Hist115 and stat230)</t>
   </si>
 </sst>
 </file>
@@ -568,20 +568,20 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="2.1328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="43.1328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="27.59765625" customWidth="1"/>
+    <col min="6" max="6" width="31.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,7 +599,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -610,7 +610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -621,7 +621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -632,7 +632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -648,7 +648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -656,7 +656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -667,7 +667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -678,7 +678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -689,7 +689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -700,7 +700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -711,7 +711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -722,7 +722,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -736,7 +736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -747,7 +747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -761,7 +761,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -772,7 +772,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -786,7 +786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -797,7 +797,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -811,7 +811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
@@ -822,7 +822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
@@ -833,7 +833,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
@@ -847,7 +847,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>45439</v>
       </c>
@@ -858,7 +858,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>45440</v>
       </c>
@@ -869,12 +869,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>45441</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
tried structure learning algorithms on variable selection, no luck
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C08764F-8A8F-4629-BCF6-7F30DC30F9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBDF17B-D1B7-4ED1-8255-1C02B946101A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,7 +154,7 @@
     <t>Imputation into random forest seems to work the best…</t>
   </si>
   <si>
-    <t>Meeting. Tried pairwise correlation, high cor on odd subjects (eg. Hist115 and stat230)</t>
+    <t>Meeting. Tried pairwise correlation, high cor on odd subjects (eg. Hist115 and stat230). Structured learning algorithms don’t seem to be finding any worthwhile connections</t>
   </si>
 </sst>
 </file>
@@ -568,20 +568,20 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.86328125" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" customWidth="1"/>
-    <col min="3" max="3" width="2.1328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.1328125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27.59765625" customWidth="1"/>
-    <col min="6" max="6" width="31.265625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,7 +599,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -610,7 +610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -621,7 +621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -632,7 +632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -648,7 +648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -656,7 +656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -667,7 +667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -678,7 +678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -689,7 +689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -700,7 +700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -711,7 +711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -722,7 +722,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -736,7 +736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -747,7 +747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -761,7 +761,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -772,7 +772,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -786,7 +786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -797,7 +797,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -811,7 +811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
@@ -822,7 +822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
@@ -833,7 +833,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
@@ -847,7 +847,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>45439</v>
       </c>
@@ -858,7 +858,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>45440</v>
       </c>
@@ -869,12 +869,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>45441</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
starting new rmd on GBMs
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0659724-B1B5-4F60-8A6D-6FB2CE9A5BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E715667F-42AA-43B2-A933-A0000476A12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Workday courses. Looked into SVM, going to have to change how the data is formatted. Now looking for more feature selection models (gbm somehow works)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading papers on feature selection. Lasso, </t>
+  </si>
+  <si>
+    <t>Regroup w Daniel. Starting new rmd on GBMs</t>
   </si>
 </sst>
 </file>
@@ -568,23 +574,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="2.1328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="43.1328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="27.59765625" customWidth="1"/>
+    <col min="6" max="6" width="31.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -613,7 +619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -624,7 +630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -635,7 +641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -643,7 +649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -651,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -659,7 +665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -670,7 +676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -681,7 +687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -692,7 +698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -703,7 +709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -714,7 +720,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -725,7 +731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -739,7 +745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -750,7 +756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -764,7 +770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -775,7 +781,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -789,7 +795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -800,7 +806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -814,7 +820,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
@@ -825,7 +831,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
@@ -836,7 +842,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
@@ -850,7 +856,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>45439</v>
       </c>
@@ -861,7 +867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>45440</v>
       </c>
@@ -872,7 +878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>45441</v>
       </c>
@@ -883,7 +889,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>45442</v>
       </c>
@@ -894,12 +900,26 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>45443</v>
       </c>
       <c r="B28">
         <v>4</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="4">
+        <v>45446</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grid search on gbm and error bars added
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36112AD-9B10-4A31-B08E-29F726612990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B4230E-6252-495C-A28B-00C39D2E6E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -207,6 +207,27 @@
   </si>
   <si>
     <t>Regroup w Daniel. Starting new rmd on GBMs, regression works, classification has some weird results</t>
+  </si>
+  <si>
+    <t>Day of week</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Sorting code for meeting, meeting, grid search of parameters, added 95% CI error bars to predictions graph</t>
   </si>
 </sst>
 </file>
@@ -617,352 +638,434 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="2.73046875" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" customWidth="1"/>
+    <col min="4" max="4" width="2.1328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="43.1328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.59765625" customWidth="1"/>
+    <col min="7" max="7" width="31.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4"/>
+      <c r="C2">
         <v>1.5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4"/>
+      <c r="C3">
         <v>0.5</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4"/>
+      <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4"/>
+      <c r="C5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4"/>
+      <c r="C6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4"/>
+      <c r="C7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4"/>
+      <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4"/>
+      <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4"/>
+      <c r="C10">
         <v>4</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4"/>
+      <c r="C11">
         <v>6</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12">
         <v>6</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13">
         <v>8</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14">
         <v>8</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15">
         <v>6</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16">
         <v>6</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18">
         <v>4</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19">
         <v>8</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20">
         <v>6</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21">
         <v>7</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22">
         <v>7</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23">
         <v>3</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>45439</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24">
         <v>8</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>45440</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25">
         <v>8</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>45441</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26">
         <v>8</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>45442</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27">
         <v>7</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>45443</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28">
         <v>4</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>45446</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29">
         <v>8</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A30" s="4">
+        <v>45447</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -980,15 +1083,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1002,7 +1105,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -1013,7 +1116,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -1024,7 +1127,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>45</v>
       </c>
@@ -1032,7 +1135,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
xgboost and gridsearch added
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8952C05-1B4A-4E69-8ED0-09D2270354FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A05353E-3721-442C-B792-8328F087D29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>Revisiting error bars, very small. Reviewing xgboost and different loss functions to implement. Looking into why data is predicted in such a small range + graphing it</t>
+  </si>
+  <si>
+    <t>want to run grid search on xgboost</t>
+  </si>
+  <si>
+    <t>Meeting, using quantile regression for error bars. Xgboost is working, grid search on xgboost</t>
   </si>
 </sst>
 </file>
@@ -644,7 +650,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
@@ -1100,6 +1106,23 @@
       </c>
       <c r="E32" s="5" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A33" s="4">
+        <v>45454</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added low grades back in with error bars
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A05353E-3721-442C-B792-8328F087D29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4373FF82-659A-4468-B918-0902251B18D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>Meeting, using quantile regression for error bars. Xgboost is working, grid search on xgboost</t>
+  </si>
+  <si>
+    <t>Still running grid search, added back in grades &lt; 60. Removing rows without prereqs helped a bunch on train/test. Quantile error bars look good w new data</t>
   </si>
 </sst>
 </file>
@@ -650,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1123,6 +1126,20 @@
       </c>
       <c r="G33" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A34" s="4">
+        <v>45455</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bootstrap error bars on xgb
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4373FF82-659A-4468-B918-0902251B18D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D9539B-0CAC-4CC4-BD18-4AEA2BBB4D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -242,7 +242,10 @@
     <t>Meeting, using quantile regression for error bars. Xgboost is working, grid search on xgboost</t>
   </si>
   <si>
-    <t>Still running grid search, added back in grades &lt; 60. Removing rows without prereqs helped a bunch on train/test. Quantile error bars look good w new data</t>
+    <t>Still running grid search, added back in grades &lt; 60. Removing rows without prereqs helped a bunch on train/test. Quantile error bars look good w new data. Bootstrap error bars on xgboost</t>
+  </si>
+  <si>
+    <t>should play around with bootstrapping more</t>
   </si>
 </sst>
 </file>
@@ -653,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1128,7 +1131,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>45455</v>
       </c>
@@ -1136,10 +1139,15 @@
         <v>53</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G35" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on adding profs to prediction
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23705E65-8A9F-47B9-9CA2-39694FC69DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3009E9A5-5941-4DE2-9448-D28D96A22C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -668,21 +668,21 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.86328125" customWidth="1"/>
-    <col min="2" max="2" width="2.73046875" customWidth="1"/>
-    <col min="3" max="3" width="11.59765625" customWidth="1"/>
-    <col min="4" max="4" width="2.1328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="43.1328125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="27.59765625" customWidth="1"/>
-    <col min="7" max="7" width="31.265625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="43.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +703,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -715,7 +715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -727,7 +727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -739,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -748,7 +748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -757,7 +757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -766,7 +766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -778,7 +778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -790,7 +790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -802,7 +802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -814,7 +814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -828,7 +828,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -842,7 +842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -859,7 +859,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -873,7 +873,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -890,7 +890,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -904,7 +904,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -921,7 +921,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -935,7 +935,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -952,7 +952,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
@@ -966,7 +966,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
@@ -980,7 +980,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
@@ -997,7 +997,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>45439</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>45440</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>45441</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>45442</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>45443</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>45446</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>45447</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>45448</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>45453</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>45454</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>45455</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>45456</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>45457</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>52</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>64</v>
@@ -1203,15 +1203,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>45</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
making vector of profs
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3009E9A5-5941-4DE2-9448-D28D96A22C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40D8E2E-156A-476F-8DC8-6AC626DE958B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -255,6 +255,15 @@
   </si>
   <si>
     <t>adding more prediction data: professors, majors and minors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database manipulation and </t>
+  </si>
+  <si>
+    <t>need to make length of student major minors equal to the length of unique student ids, then join. Probably can just use NA skip over profs who wont exist…</t>
+  </si>
+  <si>
+    <t>trying to mesh profs onto main df_bsc table</t>
   </si>
 </sst>
 </file>
@@ -665,24 +674,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="2.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="2.73046875" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" customWidth="1"/>
+    <col min="4" max="4" width="2.1328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="43.1328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.59765625" customWidth="1"/>
+    <col min="7" max="7" width="31.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +712,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -715,7 +724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -727,7 +736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -739,7 +748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -748,7 +757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -757,7 +766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -766,7 +775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -778,7 +787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -790,7 +799,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -802,7 +811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -814,7 +823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -828,7 +837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -842,7 +851,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -859,7 +868,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -873,7 +882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -890,7 +899,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -904,7 +913,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -921,7 +930,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -935,7 +944,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -952,7 +961,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
@@ -966,7 +975,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
@@ -980,7 +989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
@@ -997,7 +1006,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>45439</v>
       </c>
@@ -1011,7 +1020,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>45440</v>
       </c>
@@ -1025,7 +1034,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>45441</v>
       </c>
@@ -1039,7 +1048,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>45442</v>
       </c>
@@ -1053,7 +1062,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>45443</v>
       </c>
@@ -1067,7 +1076,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>45446</v>
       </c>
@@ -1081,7 +1090,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>45447</v>
       </c>
@@ -1095,7 +1104,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
         <v>45448</v>
       </c>
@@ -1109,7 +1118,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
         <v>45453</v>
       </c>
@@ -1123,7 +1132,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
         <v>45454</v>
       </c>
@@ -1140,7 +1149,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>45455</v>
       </c>
@@ -1154,7 +1163,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
         <v>45456</v>
       </c>
@@ -1171,7 +1180,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
         <v>45457</v>
       </c>
@@ -1186,6 +1195,37 @@
       </c>
       <c r="G36" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="4">
+        <v>45460</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="4">
+        <v>45461</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1203,15 +1243,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1225,7 +1265,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -1236,7 +1276,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -1247,7 +1287,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>45</v>
       </c>
@@ -1255,7 +1295,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
adjusted majors to match studentID length
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40D8E2E-156A-476F-8DC8-6AC626DE958B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E6EBCE-72AB-4EFC-96E6-15C456B0AD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>trying to mesh profs onto main df_bsc table</t>
+  </si>
+  <si>
+    <t>organizing things for email update, reading papers on different methods of GBM implementation and variations. Saving profs to studentgrades_prof</t>
   </si>
 </sst>
 </file>
@@ -674,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -689,6 +692,11 @@
     <col min="5" max="5" width="43.1328125" style="5" customWidth="1"/>
     <col min="6" max="6" width="27.59765625" customWidth="1"/>
     <col min="7" max="7" width="31.265625" customWidth="1"/>
+    <col min="24" max="25" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -1226,6 +1234,20 @@
       </c>
       <c r="G38" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A39" s="4">
+        <v>45463</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
studentgrades_prof test group data created
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E6EBCE-72AB-4EFC-96E6-15C456B0AD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5F440F-E21D-431F-AECD-31414D758DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>organizing things for email update, reading papers on different methods of GBM implementation and variations. Saving profs to studentgrades_prof</t>
+  </si>
+  <si>
+    <t>Finished creating studentgrades_prof for test group</t>
   </si>
 </sst>
 </file>
@@ -677,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1248,6 +1251,20 @@
       </c>
       <c r="E39" s="5" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="4">
+        <v>45464</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40">
+        <v>0.5</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding professor columns to all courses
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B31283-5D8E-4F34-99E2-5405C4F21759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F267956E-5085-41DE-AC12-A1BE42010593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>paper review, code organization, plan for future steps</t>
+  </si>
+  <si>
+    <t>cleaning professors table, merging professors into main students dataframe</t>
   </si>
 </sst>
 </file>
@@ -683,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1282,6 +1285,20 @@
       </c>
       <c r="E41" s="5" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A42" s="4">
+        <v>45474</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed prof column removal
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F267956E-5085-41DE-AC12-A1BE42010593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385C5105-C796-4CC6-B5D0-4CF69516EDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>cleaning professors table, merging professors into main students dataframe</t>
+  </si>
+  <si>
+    <t>finalizing studentgrades_prof, cleaning out irrelevant prof columns</t>
+  </si>
+  <si>
+    <t>running GBM with different configurations, fixing prof column removal, adding recursive removal to columns to improve prediction</t>
   </si>
 </sst>
 </file>
@@ -686,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1299,6 +1305,34 @@
       </c>
       <c r="E42" s="5" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A43" s="4">
+        <v>45475</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A44" s="4">
+        <v>45476</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing different courses, looking at letter grades
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73620495-955E-4AE5-AA10-37A63FAAB701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FF4F69-2AC1-4A2D-A81A-54A87A273F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -284,10 +284,10 @@
     <t>running GBM with different configurations, fixing prof column removal, adding recursive removal to columns to improve prediction</t>
   </si>
   <si>
-    <t>Implementing some variable selection.. Doesn't seem to improve model</t>
-  </si>
-  <si>
     <t>want to see what happens when predicting single students</t>
+  </si>
+  <si>
+    <t>Implementing some variable selection.. Doesn't seem to improve model, trying different courses (seem to need more data), trying a categorical letter grade prediction on students</t>
   </si>
 </sst>
 </file>
@@ -701,7 +701,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1341,7 +1341,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
         <v>45477</v>
       </c>
@@ -1349,13 +1349,13 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E45" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G45" t="s">
         <v>74</v>
-      </c>
-      <c r="G45" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created new rmd summarizing all work so far
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC64D8E1-9FA9-4558-B371-964740ED1B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8D86EA-FE99-4724-B6A6-BA084E7F56EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,10 +293,10 @@
     <t>set up heat map for letter grade prediction, changing several variables to check improvement (train/test ratio, necessary pre reqs, # of Nas allowed in columns)</t>
   </si>
   <si>
-    <t>organizing data for meeting, meeting</t>
-  </si>
-  <si>
     <t>creating a new markdown with entire workflow: loading data, processing data, training model, results</t>
+  </si>
+  <si>
+    <t>organizing data for meeting, meeting, structuring new rmd with all work completed this summer, adding student grades code</t>
   </si>
 </sst>
 </file>
@@ -709,27 +709,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="2.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1"/>
-    <col min="24" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="2.73046875" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" customWidth="1"/>
+    <col min="4" max="4" width="2.1328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="43.1328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.59765625" customWidth="1"/>
+    <col min="7" max="7" width="31.265625" customWidth="1"/>
+    <col min="24" max="25" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -750,7 +750,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -762,7 +762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -774,7 +774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -786,7 +786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -795,7 +795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -804,7 +804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -813,7 +813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -825,7 +825,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -837,7 +837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -849,7 +849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -861,7 +861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -875,7 +875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -889,7 +889,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -906,7 +906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -920,7 +920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -937,7 +937,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -951,7 +951,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -968,7 +968,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -982,7 +982,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -999,7 +999,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>45439</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>45440</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>45441</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>45442</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>45443</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>45446</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>45447</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
         <v>45448</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
         <v>45453</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
         <v>45454</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>45455</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
         <v>45456</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
         <v>45457</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>45460</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>45461</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
         <v>45463</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="4">
         <v>45464</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="4">
         <v>45465</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="4">
         <v>45474</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="4">
         <v>45475</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A44" s="4">
         <v>45476</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
         <v>45477</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
         <v>45478</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A47" s="4">
         <v>45483</v>
       </c>
@@ -1389,13 +1389,13 @@
         <v>53</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E47" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G47" t="s">
         <v>77</v>
-      </c>
-      <c r="G47" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1413,15 +1413,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>45</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
added more code and text to compile rmd
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8D86EA-FE99-4724-B6A6-BA084E7F56EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CB0829-5FB8-4433-8E00-B1A64E47927A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>organizing data for meeting, meeting, structuring new rmd with all work completed this summer, adding student grades code</t>
+  </si>
+  <si>
+    <t>working on compiling all code, considering adjusting student grades to either: two different named dfs, or altering the structure of .1 .2 to accommodate other code (would be more work but we can use first attempt data easily)</t>
   </si>
 </sst>
 </file>
@@ -707,29 +710,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.86328125" customWidth="1"/>
-    <col min="2" max="2" width="2.73046875" customWidth="1"/>
-    <col min="3" max="3" width="11.59765625" customWidth="1"/>
-    <col min="4" max="4" width="2.1328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="43.1328125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="27.59765625" customWidth="1"/>
-    <col min="7" max="7" width="31.265625" customWidth="1"/>
-    <col min="24" max="25" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="43.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" customWidth="1"/>
+    <col min="24" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -750,7 +753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -762,7 +765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -774,7 +777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -786,7 +789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -795,7 +798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -804,7 +807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -813,7 +816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -825,7 +828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -837,7 +840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -849,7 +852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -861,7 +864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -875,7 +878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -889,7 +892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -906,7 +909,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -920,7 +923,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -937,7 +940,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -951,7 +954,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -968,7 +971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -982,7 +985,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -999,7 +1002,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>45439</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>45440</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>45441</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>45442</v>
       </c>
@@ -1100,7 +1103,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>45443</v>
       </c>
@@ -1114,7 +1117,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>45446</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>45447</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>45448</v>
       </c>
@@ -1156,7 +1159,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>45453</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>45454</v>
       </c>
@@ -1187,7 +1190,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>45455</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>45456</v>
       </c>
@@ -1218,7 +1221,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>45457</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>45460</v>
       </c>
@@ -1249,7 +1252,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>45461</v>
       </c>
@@ -1266,7 +1269,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>45463</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>45464</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>45465</v>
       </c>
@@ -1308,7 +1311,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>45474</v>
       </c>
@@ -1322,7 +1325,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>45475</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>45476</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>45477</v>
       </c>
@@ -1367,7 +1370,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45478</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45483</v>
       </c>
@@ -1396,6 +1399,20 @@
       </c>
       <c r="G47" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>45484</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1413,15 +1430,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1435,7 +1452,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -1446,7 +1463,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -1457,7 +1474,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>45</v>
       </c>
@@ -1465,7 +1482,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
finished commenting compilation, ensuring it knits still
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8C0C22-ED0B-4450-B453-97A99E72E983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B347C1B-B990-4CB3-8E05-72956B927432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -309,6 +309,12 @@
   </si>
   <si>
     <t>Finished compiling code, drawn out rmd structure, started commenting</t>
+  </si>
+  <si>
+    <t>Differentiated the three studentgrades (_rep and _prof). Started commenting code, some revising on code.</t>
+  </si>
+  <si>
+    <t>Finished commenting code. Ensuring it runs/knits correctly. Need to finish up error bar section, RFE, and xgbms</t>
   </si>
 </sst>
 </file>
@@ -719,29 +725,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="2.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1"/>
-    <col min="24" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="2.73046875" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" customWidth="1"/>
+    <col min="4" max="4" width="2.1328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="43.1328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.59765625" customWidth="1"/>
+    <col min="7" max="7" width="31.265625" customWidth="1"/>
+    <col min="24" max="25" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,7 +768,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -774,7 +780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -786,7 +792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -798,7 +804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -807,7 +813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -816,7 +822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -825,7 +831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -837,7 +843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -849,7 +855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -861,7 +867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -873,7 +879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -887,7 +893,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -901,7 +907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -918,7 +924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -932,7 +938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -949,7 +955,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -963,7 +969,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -980,7 +986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -994,7 +1000,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -1011,7 +1017,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
@@ -1025,7 +1031,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
@@ -1039,7 +1045,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>45439</v>
       </c>
@@ -1070,7 +1076,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>45440</v>
       </c>
@@ -1084,7 +1090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>45441</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>45442</v>
       </c>
@@ -1112,7 +1118,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>45443</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>45446</v>
       </c>
@@ -1140,7 +1146,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>45447</v>
       </c>
@@ -1154,7 +1160,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
         <v>45448</v>
       </c>
@@ -1168,7 +1174,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
         <v>45453</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
         <v>45454</v>
       </c>
@@ -1199,7 +1205,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>45455</v>
       </c>
@@ -1213,7 +1219,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
         <v>45456</v>
       </c>
@@ -1230,7 +1236,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
         <v>45457</v>
       </c>
@@ -1247,7 +1253,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>45460</v>
       </c>
@@ -1261,7 +1267,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>45461</v>
       </c>
@@ -1278,7 +1284,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
         <v>45463</v>
       </c>
@@ -1292,7 +1298,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="4">
         <v>45464</v>
       </c>
@@ -1306,7 +1312,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="4">
         <v>45465</v>
       </c>
@@ -1320,7 +1326,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="4">
         <v>45474</v>
       </c>
@@ -1334,7 +1340,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="4">
         <v>45475</v>
       </c>
@@ -1348,7 +1354,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A44" s="4">
         <v>45476</v>
       </c>
@@ -1362,7 +1368,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
         <v>45477</v>
       </c>
@@ -1379,7 +1385,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
         <v>45478</v>
       </c>
@@ -1393,7 +1399,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A47" s="4">
         <v>45483</v>
       </c>
@@ -1410,7 +1416,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A48" s="4">
         <v>45484</v>
       </c>
@@ -1424,7 +1430,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A49" s="4">
         <v>45485</v>
       </c>
@@ -1438,7 +1444,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A50" s="4">
         <v>45486</v>
       </c>
@@ -1455,15 +1461,32 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A51" s="4">
+        <v>45487</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A52" s="4">
         <v>45488</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C51">
-        <v>2</v>
+      <c r="C52">
+        <v>8</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1481,15 +1504,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1503,7 +1526,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -1514,7 +1537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -1525,7 +1548,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>45</v>
       </c>
@@ -1533,7 +1556,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
finished commenting code compilation
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B347C1B-B990-4CB3-8E05-72956B927432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF7B4AB-A72D-43EF-A4CD-20E3FA0AADCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -725,29 +725,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.86328125" customWidth="1"/>
-    <col min="2" max="2" width="2.73046875" customWidth="1"/>
-    <col min="3" max="3" width="11.59765625" customWidth="1"/>
-    <col min="4" max="4" width="2.1328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="43.1328125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="27.59765625" customWidth="1"/>
-    <col min="7" max="7" width="31.265625" customWidth="1"/>
-    <col min="24" max="25" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="43.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" customWidth="1"/>
+    <col min="24" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -768,7 +768,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -780,7 +780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -792,7 +792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -804,7 +804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -813,7 +813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -822,7 +822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -831,7 +831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -843,7 +843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -855,7 +855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -867,7 +867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -879,7 +879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -893,7 +893,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -907,7 +907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -924,7 +924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -938,7 +938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -955,7 +955,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -969,7 +969,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -986,7 +986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>45439</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>45440</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>45441</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>45442</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>45443</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>45446</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>45447</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>45448</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>45453</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>45454</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>45455</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>45456</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>45457</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>45460</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>45461</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>45463</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>45464</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>45465</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>45474</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>45475</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>45476</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>45477</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45478</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45483</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>45484</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>45485</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>45486</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>45487</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>45488</v>
       </c>
@@ -1487,6 +1487,14 @@
       </c>
       <c r="E52" s="5" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>45489</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1504,15 +1512,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1526,7 +1534,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -1537,7 +1545,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -1548,7 +1556,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>45</v>
       </c>
@@ -1556,7 +1564,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
new data incorporated into studentgrades
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBEFEC0-1E65-47C7-A48D-03375BB0ECA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316C0249-0181-470A-871E-2486ADDE1A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -323,7 +323,13 @@
     <t>Doing more exploring into the new data…. There are not nearly enough rows… will email irene</t>
   </si>
   <si>
-    <t>Compiled all old data with new data (excluding overlap).</t>
+    <t>Compiled all old data with new data (excluding overlap). Running and testing old code with new dataset, everything working fine</t>
+  </si>
+  <si>
+    <t>implementing residency, gender, citizenship. Have to rewrite and recompile new rows into old df to include gender etc.</t>
+  </si>
+  <si>
+    <t>added new rows to both studentgrades and studentgrades_prof. new columns for new variables. Doesn't seem to be helping, in fact performing worse… need to debug</t>
   </si>
 </sst>
 </file>
@@ -734,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,7 +1532,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>45491</v>
       </c>
@@ -1534,18 +1540,38 @@
         <v>50</v>
       </c>
       <c r="C55">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>45492</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>52</v>
+      </c>
+      <c r="C56">
+        <v>8</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>45495</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new student rows, added gender etc. to studentgrades
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316C0249-0181-470A-871E-2486ADDE1A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8694BDEB-0F10-4264-9ACA-8A6BC66B5BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -329,7 +329,7 @@
     <t>implementing residency, gender, citizenship. Have to rewrite and recompile new rows into old df to include gender etc.</t>
   </si>
   <si>
-    <t>added new rows to both studentgrades and studentgrades_prof. new columns for new variables. Doesn't seem to be helping, in fact performing worse… need to debug</t>
+    <t>added new rows to both studentgrades and studentgrades_prof. new columns for new variables. Doesn't seem to be helping, in fact performing worse… need to debug, can't tell if it’s the new student affecting prediction…</t>
   </si>
 </sst>
 </file>
@@ -743,7 +743,7 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,7 +1560,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>45495</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>51</v>
       </c>
       <c r="C57">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
testing imputation models on studentgrades_prof
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735496EE-2F51-4397-A454-72C021C6920B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA0A87A-6A7D-4739-8199-1C65327EAB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>making GBMs work on the 4 dataset variations:     setting up dataframe to collect all rmse, kitting to html</t>
+  </si>
+  <si>
+    <t>Cleaning up graph comparing models, sent email, reading up on imputation</t>
+  </si>
+  <si>
+    <t>Testing studentgrades_prof with imputation again, on all courses used in GBM</t>
   </si>
 </sst>
 </file>
@@ -752,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,6 +1621,34 @@
       </c>
       <c r="F59" s="7" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>45498</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>45499</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
missForest imputation no good
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA0A87A-6A7D-4739-8199-1C65327EAB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8ED9D9-3261-48F5-B98E-49E5BAF1586D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t>Testing studentgrades_prof with imputation again, on all courses used in GBM</t>
+  </si>
+  <si>
+    <t>Reviewing the imputation methods, found out we were leaking grades into prediction variables so those methods cannot be used. Looking into the possibility of neural nets for prediction</t>
   </si>
 </sst>
 </file>
@@ -758,29 +761,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="2.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1"/>
-    <col min="24" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="2.73046875" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" customWidth="1"/>
+    <col min="4" max="4" width="2.1328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="43.1328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.59765625" customWidth="1"/>
+    <col min="7" max="7" width="31.265625" customWidth="1"/>
+    <col min="24" max="25" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,7 +804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>45407</v>
       </c>
@@ -813,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>45412</v>
       </c>
@@ -825,7 +828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>45414</v>
       </c>
@@ -837,7 +840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>45415</v>
       </c>
@@ -846,7 +849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>45417</v>
       </c>
@@ -855,7 +858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>45418</v>
       </c>
@@ -864,7 +867,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>45419</v>
       </c>
@@ -876,7 +879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>45420</v>
       </c>
@@ -888,7 +891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>45421</v>
       </c>
@@ -900,7 +903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>45422</v>
       </c>
@@ -912,7 +915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>45425</v>
       </c>
@@ -926,7 +929,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>45426</v>
       </c>
@@ -940,7 +943,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>45427</v>
       </c>
@@ -957,7 +960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>45428</v>
       </c>
@@ -971,7 +974,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>45429</v>
       </c>
@@ -988,7 +991,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>45430</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>45431</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>45433</v>
       </c>
@@ -1033,7 +1036,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>45434</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>45435</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>45436</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>45438</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>45439</v>
       </c>
@@ -1109,7 +1112,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>45440</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>45441</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>45442</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>45443</v>
       </c>
@@ -1165,7 +1168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>45446</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>45447</v>
       </c>
@@ -1193,7 +1196,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
         <v>45448</v>
       </c>
@@ -1207,7 +1210,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
         <v>45453</v>
       </c>
@@ -1221,7 +1224,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
         <v>45454</v>
       </c>
@@ -1238,7 +1241,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>45455</v>
       </c>
@@ -1252,7 +1255,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
         <v>45456</v>
       </c>
@@ -1269,7 +1272,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
         <v>45457</v>
       </c>
@@ -1286,7 +1289,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>45460</v>
       </c>
@@ -1300,7 +1303,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>45461</v>
       </c>
@@ -1317,7 +1320,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
         <v>45463</v>
       </c>
@@ -1331,7 +1334,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="4">
         <v>45464</v>
       </c>
@@ -1345,7 +1348,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="4">
         <v>45465</v>
       </c>
@@ -1359,7 +1362,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="4">
         <v>45474</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="4">
         <v>45475</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A44" s="4">
         <v>45476</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
         <v>45477</v>
       </c>
@@ -1418,7 +1421,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
         <v>45478</v>
       </c>
@@ -1432,7 +1435,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A47" s="4">
         <v>45483</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A48" s="4">
         <v>45484</v>
       </c>
@@ -1463,7 +1466,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A49" s="4">
         <v>45485</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A50" s="4">
         <v>45486</v>
       </c>
@@ -1494,7 +1497,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A51" s="4">
         <v>45487</v>
       </c>
@@ -1508,7 +1511,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A52" s="4">
         <v>45488</v>
       </c>
@@ -1522,7 +1525,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A53" s="4">
         <v>45489</v>
       </c>
@@ -1536,7 +1539,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A54" s="4">
         <v>45490</v>
       </c>
@@ -1550,7 +1553,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A55" s="4">
         <v>45491</v>
       </c>
@@ -1564,7 +1567,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A56" s="4">
         <v>45492</v>
       </c>
@@ -1578,7 +1581,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A57" s="4">
         <v>45495</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A58" s="4">
         <v>45496</v>
       </c>
@@ -1606,7 +1609,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A59" s="4">
         <v>45497</v>
       </c>
@@ -1623,7 +1626,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A60" s="4">
         <v>45498</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A61" s="4">
         <v>45499</v>
       </c>
@@ -1649,6 +1652,20 @@
       </c>
       <c r="E61" s="5" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="A62" s="4">
+        <v>45502</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C62">
+        <v>6</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1666,15 +1683,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1688,7 +1705,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -1699,7 +1716,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -1710,7 +1727,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>45</v>
       </c>
@@ -1718,7 +1735,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
pushing work from weekend
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossc\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B9DF5C-B97D-4D9A-BA01-B667E542325B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6769A164-1062-4C9D-9FC4-3E85D5F039D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -348,6 +348,18 @@
   </si>
   <si>
     <t>Reviewing the imputation methods, found out we were leaking grades into prediction variables so those methods cannot be used. Looking into the possibility of neural nets for prediction</t>
+  </si>
+  <si>
+    <t>Building datasets for COSC 221, DATA 301 &amp; 311. Used STAT 230 too. Built grid search to find patterns between best hyperparameters. Started code</t>
+  </si>
+  <si>
+    <t>A lower shrinkage rate and slightly higher interacton depth performed better,  Minimum number of observations in terminal nodes (n.minobsinnode) seemed to move around with no pattern. Repeated for STAT 303 and MATH 221</t>
+  </si>
+  <si>
+    <t>MATH 221 didn't seem to perform well depite having the most students having taken the course. Doing separate testing on on MATH 221 on the main function to see if the setup isn't working.</t>
+  </si>
+  <si>
+    <t>Re running  grid search on all datasets and re evaluating RMSEs. The RMSEs dropped 0.5-1 for each of the courses and similar observations with hyperparameters were found.</t>
   </si>
 </sst>
 </file>
@@ -761,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1666,6 +1678,62 @@
       </c>
       <c r="E62" s="5" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A63" s="4">
+        <v>45504</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A64" s="4">
+        <v>45505</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A65" s="4">
+        <v>45507</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A66" s="4">
+        <v>45509</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pytorch cnn model to repo
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2570D3-F628-4AEC-92B9-59DEACDB2DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0ED200-9F94-429B-9B1E-74F623256BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="104">
   <si>
     <t>Date</t>
   </si>
@@ -363,6 +363,15 @@
   </si>
   <si>
     <t>Setting up CUDA and environment for neural networks. This was done in python 3.12.4 and torch 2.4.0 (pytorch). Created a new base dataset using the original raw data with professors. A Long Short Term Memory model was used to feed in the data row by row.</t>
+  </si>
+  <si>
+    <t>Debugging and trying to format data into model. Need to factor everything and push as ints.</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/figure/Model-description-of-the-hybrid-2D-CNN-Model_fig1_359461812</t>
+  </si>
+  <si>
+    <t>Saved a factored model to use in pytorch. Reading research papers on CNNs use in grade prediction. Set up and run custom CNNs on grades. Haven't set up certain courses yet.</t>
   </si>
 </sst>
 </file>
@@ -776,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,7 +1720,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>45507</v>
       </c>
@@ -1725,7 +1734,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>45509</v>
       </c>
@@ -1739,7 +1748,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>45510</v>
       </c>
@@ -1751,6 +1760,37 @@
       </c>
       <c r="E67" s="5" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>45511</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>45512</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C69">
+        <v>8</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F69" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before the big cleanup
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5D17CE-C4B7-4373-B497-E7753C66FB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6ECFAE-325B-4EEB-BDEF-13FEAE45BC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -378,6 +378,12 @@
   </si>
   <si>
     <t>Built two models. A simple linear model, and a CNN. Changing and designing train/test sets for different subjects.</t>
+  </si>
+  <si>
+    <t>Changed train/val/test sets to be 10% of course we're trying to predict on for each of validation and testing, and the rest of the rows were used for training. Implemented the model from the paper, and a simple sequential model. Sequential was same as linear model performance and all. The model from the paper performed the best</t>
+  </si>
+  <si>
+    <t>change training set to only have student's grades who have taken the course we're trying to predict on</t>
   </si>
 </sst>
 </file>
@@ -791,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,7 +1732,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>45507</v>
       </c>
@@ -1740,7 +1746,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>45509</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>45510</v>
       </c>
@@ -1768,7 +1774,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>45511</v>
       </c>
@@ -1782,7 +1788,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>45512</v>
       </c>
@@ -1799,7 +1805,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>45514</v>
       </c>
@@ -1813,7 +1819,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>45515</v>
       </c>
@@ -1825,6 +1831,23 @@
       </c>
       <c r="E71" s="5" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>45516</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72">
+        <v>6</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaning up knitted file
</commit_message>
<xml_diff>
--- a/Summer 2024 Working Hours.xlsx
+++ b/Summer 2024 Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\UBCO-Grade-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6ECFAE-325B-4EEB-BDEF-13FEAE45BC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A51FA9F-1462-4E14-A9ED-96A1CE1FBA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1F181F4-7687-440B-825F-2C207C6D6F7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -384,6 +384,12 @@
   </si>
   <si>
     <t>change training set to only have student's grades who have taken the course we're trying to predict on</t>
+  </si>
+  <si>
+    <t>Editting the rmd file and knitting. Corrections include: adding links to data and models, adding graphs for each model, cleaning up and displaying all dataset formats, reducing output overall to only include relevant information.</t>
+  </si>
+  <si>
+    <t>text for results, organize rdata files to folder, add a description to the github</t>
   </si>
 </sst>
 </file>
@@ -448,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -462,6 +468,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -797,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A58F2-8B3E-430D-B398-5A920816A326}">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="L69" sqref="L69"/>
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,7 +1859,39 @@
         <v>107</v>
       </c>
     </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>45519</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C73">
+        <v>6</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>45520</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C74">
+        <v>8</v>
+      </c>
+      <c r="E74" s="8"/>
+      <c r="G74" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E73:E74"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>